<commit_message>
:wrench: updates meta lookup with the categories produced by sheila and shaurya
</commit_message>
<xml_diff>
--- a/data/project/tt_meta_project_lu.xlsx
+++ b/data/project/tt_meta_project_lu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/talking_therapies-1/data/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7AC13A0-2FDA-41ED-90C0-EE9607056F25}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBC150E4-4992-40B6-89DE-AF66D1741F44}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="3840" windowWidth="21090" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15645" yWindow="1080" windowWidth="13260" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lu" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>file</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>NHS Talking Therapies NELFT</t>
+  </si>
+  <si>
+    <t>Multi-component (informational and operational)</t>
+  </si>
+  <si>
+    <t>Informational</t>
+  </si>
+  <si>
+    <t>plymouth</t>
+  </si>
+  <si>
+    <t>dr_julian</t>
   </si>
 </sst>
 </file>
@@ -131,8 +143,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9B7D47F6-24FA-41FA-AC6F-8ED09663437B}" name="file"/>
     <tableColumn id="2" xr3:uid="{B85DCA2B-34BB-46A2-97CC-3B964A62CEFA}" name="name_full"/>
@@ -405,17 +417,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -436,6 +448,9 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -444,6 +459,9 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -452,6 +470,9 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -460,6 +481,9 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -468,6 +492,9 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -476,6 +503,9 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -483,6 +513,25 @@
       </c>
       <c r="B8" t="s">
         <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:package: updates the lookup file with the latest projects
</commit_message>
<xml_diff>
--- a/data/project/tt_meta_project_lu.xlsx
+++ b/data/project/tt_meta_project_lu.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/talking_therapies-1/data/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBC150E4-4992-40B6-89DE-AF66D1741F44}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DF3CA8B-2F44-43D6-AA9A-64AA4FFBCEAD}"/>
   <bookViews>
-    <workbookView xWindow="15645" yWindow="1080" windowWidth="13260" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="5850" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lu" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>file</t>
   </si>
@@ -54,9 +65,6 @@
     <t>NHS Cornwall and Isles of Scilly Talking Therapies</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>TALKWORKS Devon NHS Talking Therapies</t>
   </si>
   <si>
@@ -88,6 +96,30 @@
   </si>
   <si>
     <t>dr_julian</t>
+  </si>
+  <si>
+    <t>bradford</t>
+  </si>
+  <si>
+    <t>NHS Bradford District and Craven Talking Therapies</t>
+  </si>
+  <si>
+    <t>sub_component</t>
+  </si>
+  <si>
+    <t>sub_targetgroup</t>
+  </si>
+  <si>
+    <t>Subgroup-specific</t>
+  </si>
+  <si>
+    <t>Non-Targeted or Mixed</t>
+  </si>
+  <si>
+    <t>yorkshire</t>
+  </si>
+  <si>
+    <t>NHS North Yorkshire Talking Therapies</t>
   </si>
 </sst>
 </file>
@@ -143,12 +175,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{1DA1C1F5-913D-49A6-881B-A66AACBEC86A}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9B7D47F6-24FA-41FA-AC6F-8ED09663437B}" name="file"/>
     <tableColumn id="2" xr3:uid="{B85DCA2B-34BB-46A2-97CC-3B964A62CEFA}" name="name_full"/>
-    <tableColumn id="3" xr3:uid="{DC462F44-694C-4CA6-BF91-9C0B0A392D3F}" name="category"/>
+    <tableColumn id="3" xr3:uid="{DC462F44-694C-4CA6-BF91-9C0B0A392D3F}" name="sub_component"/>
+    <tableColumn id="4" xr3:uid="{B7A3F629-E01C-49EF-A552-525D1A6663A4}" name="sub_targetgroup"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,9 +461,10 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,65 +472,83 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -504,34 +556,68 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>